<commit_message>
Compiling 2015-2019 low gradient field data.
</commit_message>
<xml_diff>
--- a/data/compile_2015-2019/field_data/LGSS_16-17_MASTER_v2.xlsx
+++ b/data/compile_2015-2019/field_data/LGSS_16-17_MASTER_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmlemley\OneDrive - New York State Office of Information Technology Services\Projects\LGSS\Data\2016-2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\LGSS_scripting\lgss\data\compile_2015-2019\field_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="382" documentId="13_ncr:40009_{1D6029C4-E83B-4B52-B3AD-57CC2A8E69EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{ED3C9A49-4990-4D78-9215-730981FEA146}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BE6109-4EAD-467C-A70E-C99C8972BE87}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="10580" windowWidth="19200" windowHeight="11020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bugs" sheetId="5" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -259,7 +260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2384" uniqueCount="891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2384" uniqueCount="892">
   <si>
     <t>BAS_LOC_RM</t>
   </si>
@@ -2932,6 +2933,9 @@
   </si>
   <si>
     <t>MACROPHYTE_pct</t>
+  </si>
+  <si>
+    <t>07-HARB-0.5</t>
   </si>
 </sst>
 </file>
@@ -33327,7 +33331,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:QS95">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:QS95">
     <sortCondition ref="A6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -42666,7 +42670,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:CL35">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:CL35">
     <sortCondition ref="A6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -44771,7 +44775,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:S35">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S35">
     <sortCondition ref="A11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -52489,7 +52493,7 @@
       <c r="E245" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A2:W35">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W35">
     <sortCondition ref="E12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -53151,7 +53155,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>883</v>
+        <v>891</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -54235,7 +54239,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState columnSort="1" ref="A38:P39">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="A38:P39">
     <sortCondition ref="A38:P38"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -55051,7 +55055,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState columnSort="1" ref="A1:G35">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="A1:G35">
     <sortCondition ref="A1:G1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>